<commit_message>
Implemented owlcms:fixMerges(5, [1, 2, 3])
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/schedule/DaySchedule.xlsx
+++ b/owlcms/src/main/resources/templates/schedule/DaySchedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A579784-72EE-45D7-9184-DEE54D3CDC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33673BDD-6FF2-4B23-B216-43D6E0E1AA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,8 @@
             <rFont val="Aptos Narrow"/>
             <family val="2"/>
           </rPr>
-          <t>jx:area(lastCell="L5")</t>
+          <t>jx:area(lastCell="L5")
+owlcms:fixMerges(5, [1, 2, 3])</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
Normal comp DaySchedule sessions sorted by age group
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/schedule/DaySchedule.xlsx
+++ b/owlcms/src/main/resources/templates/schedule/DaySchedule.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60728A21-984C-47BF-A6CB-633491963BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D966181B-E78B-4E0B-8E71-7E12A9D92310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25800" yWindow="4905" windowWidth="24225" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$4:$4</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -104,7 +107,7 @@
           <t xml:space="preserve">jx:each(
   items="sessionBlock.items"
   var="session"
-  select="size(session.ageGroupInfo) &gt; 0"
+  select="size(session.ageGroupInfoByAge) &gt; 0"
   lastCell="L5"
 )
 </t>
@@ -121,7 +124,7 @@
             <family val="2"/>
           </rPr>
           <t>jx:mergeCells(
-  rows="size(session.ageGroupInfo)"
+  rows="size(session.ageGroupInfoByAge)"
   cols="1"
   lastCell="D5"
 )</t>
@@ -138,7 +141,7 @@
             <family val="2"/>
           </rPr>
           <t>jx:mergeCells(
-  rows="size(session.ageGroupInfo)"
+  rows="size(session.ageGroupInfoByAge)"
   cols="1"
   lastCell="E5"
 )</t>
@@ -155,7 +158,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">jx:mergeCells(
-  rows="size(session.ageGroupInfo)"
+  rows="size(session.ageGroupInfoByAge)"
   cols="1"
   lastCell="F5"
 )
@@ -173,7 +176,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">jx:mergeCells(
-  rows="size(session.ageGroupInfo)"
+  rows="size(session.ageGroupInfoByAge)"
   cols="1"
   lastCell="G5"
 )
@@ -191,7 +194,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">jx:each(
-  items="session.ageGroupInfo"
+  items="session.ageGroupInfoByAge"
   var="agi"
   lastCell="K5"
 )
@@ -209,7 +212,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">jx:mergeCells(
-  rows="size(session.ageGroupInfo)"
+  rows="size(session.ageGroupInfoByAge)"
   cols="1"
   lastCell="L5"
 )
@@ -284,9 +287,6 @@
     <t>${t.get("Card.entryTotal")}</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>${session.name}</t>
   </si>
   <si>
@@ -294,6 +294,9 @@
   </si>
   <si>
     <t>${t.get("BY_CATEGORY")}</t>
+  </si>
+  <si>
+    <t>${t.get("Athletes")}</t>
   </si>
 </sst>
 </file>
@@ -303,7 +306,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="ddd\ mmm\ d"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +366,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -409,9 +419,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -434,9 +441,6 @@
       <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -451,6 +455,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,6 +793,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
@@ -794,10 +805,10 @@
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="1"/>
-    <col min="2" max="2" width="0.28515625" customWidth="1"/>
+    <col min="2" max="2" width="1.42578125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="6.85546875" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" customWidth="1"/>
     <col min="9" max="9" width="10.85546875" customWidth="1"/>
@@ -806,124 +817,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="28.5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:12" ht="10.5" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" s="15" customFormat="1" ht="9" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="11" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" s="10"/>
+      <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:12" s="9" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:12" s="8" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="8" t="s">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -936,8 +947,8 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="A1:L1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="83" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>